<commit_message>
Agregué el usuario Franco
</commit_message>
<xml_diff>
--- a/Usuarios - Sector.xlsx
+++ b/Usuarios - Sector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ab3741321f372e0/Compras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ab3741321f372e0/Finnegans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{D11CB233-284E-41C3-82F4-231999D7CAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B3AE59F-7470-437D-9A98-E7F8E1A0D873}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{D11CB233-284E-41C3-82F4-231999D7CAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BAC1A02-C2F5-45F6-BE34-007266F6130A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{7B2B8AD3-5368-41AC-A65A-FA1EFCDD866B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7B2B8AD3-5368-41AC-A65A-FA1EFCDD866B}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>FACUNDO SUAREZ</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>ADRIAN LUNA</t>
+  </si>
+  <si>
+    <t>FRANCO</t>
   </si>
 </sst>
 </file>
@@ -232,26 +235,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -274,6 +268,16 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -288,9 +292,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47153145-0BCC-4AD9-A152-31CDB0D291C7}" name="Usuarios" displayName="Usuarios" ref="A1:B38" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47153145-0BCC-4AD9-A152-31CDB0D291C7}" name="Usuarios" displayName="Usuarios" ref="A1:B39" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EFA60A53-9045-4EE1-BE78-6305A43F76ED}" name="Usuario" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{EFA60A53-9045-4EE1-BE78-6305A43F76ED}" name="Usuario" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{ADA6A858-AB0F-4563-B399-CF84518594F4}" name="Sector"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -594,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525B6A07-85F2-40E9-B736-30690749E343}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,9 +914,17 @@
         <v>37</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A38">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="A2:A39">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Eliminado el usuario Franco
</commit_message>
<xml_diff>
--- a/Usuarios - Sector.xlsx
+++ b/Usuarios - Sector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ab3741321f372e0/Finnegans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{D11CB233-284E-41C3-82F4-231999D7CAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BAC1A02-C2F5-45F6-BE34-007266F6130A}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{D11CB233-284E-41C3-82F4-231999D7CAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F95EF0B1-01A6-431E-AD34-10E6E51C1C6D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7B2B8AD3-5368-41AC-A65A-FA1EFCDD866B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>FACUNDO SUAREZ</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>ADRIAN LUNA</t>
-  </si>
-  <si>
-    <t>FRANCO</t>
   </si>
 </sst>
 </file>
@@ -235,17 +232,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -268,16 +274,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -291,10 +287,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47153145-0BCC-4AD9-A152-31CDB0D291C7}" name="Usuarios" displayName="Usuarios" ref="A1:B39" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47153145-0BCC-4AD9-A152-31CDB0D291C7}" name="Usuarios" displayName="Usuarios" ref="A1:B38" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EFA60A53-9045-4EE1-BE78-6305A43F76ED}" name="Usuario" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{EFA60A53-9045-4EE1-BE78-6305A43F76ED}" name="Usuario" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{ADA6A858-AB0F-4563-B399-CF84518594F4}" name="Sector"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -598,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525B6A07-85F2-40E9-B736-30690749E343}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,17 +914,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A39">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="A2:A38">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>